<commit_message>
fin rapport + perf2
</commit_message>
<xml_diff>
--- a/audit-SEO.xlsx
+++ b/audit-SEO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Temp\Site web\Starting website\FabienD_4_19042022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{011E4427-E343-44C5-82FB-B11C59172EE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{036119E4-3237-4978-AB24-F18078D5F75B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -729,6 +729,9 @@
       <c r="D9" s="6" t="s">
         <v>40</v>
       </c>
+      <c r="E9" s="6" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
@@ -929,9 +932,7 @@
       <c r="D22" t="s">
         <v>24</v>
       </c>
-      <c r="E22" s="7" t="s">
-        <v>67</v>
-      </c>
+      <c r="E22" s="7"/>
     </row>
     <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>

</xml_diff>